<commit_message>
[Add] commandline options: --requirements-sheet-name; --requirements-id-column; --requirements-text-column
</commit_message>
<xml_diff>
--- a/VCD-Generator.Tests/Data/Requirements.xlsx
+++ b/VCD-Generator.Tests/Data/Requirements.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sgerene\Documents\15-Source-Code\VCD-Generator\VCD-Generator.Tests\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sgerene\Documents\15-Source-Code\VCD-Generator\VCD-Generator\VCD-Generator.Tests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDDCC91B-8FBE-4903-915D-685969752DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F481684-A1C8-4A6D-8CE8-D284C9649A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="requirements" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>

</xml_diff>